<commit_message>
added HPO Terms column
</commit_message>
<xml_diff>
--- a/xbrowse_server/staticfiles/upload_tables/templates/individuals.xlsx
+++ b/xbrowse_server/staticfiles/upload_tables/templates/individuals.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Family Id</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>HPO Terms</t>
   </si>
 </sst>
 </file>
@@ -371,9 +374,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -385,7 +390,7 @@
     <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,6 +411,9 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>